<commit_message>
add shareablevalueset in VS ab0d2d63ff795786a5411942641dc0f03c386c94
</commit_message>
<xml_diff>
--- a/cp-questionnaire-usecontext/ig/ValueSet-code-region-territorial-division-ror-valueset.xlsx
+++ b/cp-questionnaire-usecontext/ig/ValueSet-code-region-territorial-division-ror-valueset.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Property</t>
   </si>
@@ -61,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-24T11:45:47+00:00</t>
+    <t>2025-01-24T13:24:43+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>ValueSet regroupant des valuesets du NOS pour le code de la division territoriale</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -346,26 +349,28 @@
       <c r="A12" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" t="s" s="2">
+        <v>22</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -387,12 +392,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -414,12 +419,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -441,12 +446,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -468,12 +473,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -495,12 +500,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>